<commit_message>
format rows for input
</commit_message>
<xml_diff>
--- a/src/ACAT/grades/FA24/COMP-101_FA24_01_course_data.xlsx
+++ b/src/ACAT/grades/FA24/COMP-101_FA24_01_course_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jglossner\GitRivier\Assessment\src\ACAT\grades\FA24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E212853-CC40-4BDF-BAF2-B8F61DF27AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5953768E-BC3A-47B5-AEA1-C8079FF25B35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="525" yWindow="4335" windowWidth="21600" windowHeight="11025" xr2:uid="{3833C598-C2F8-49E4-AD33-D16D6B8DFCA6}"/>
+    <workbookView xWindow="480" yWindow="4335" windowWidth="21645" windowHeight="11025" xr2:uid="{054E22F7-75FD-4511-9B2F-9D2D4F7760FC}"/>
   </bookViews>
   <sheets>
     <sheet name="COMP-101_FA24_01_course_data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="67">
   <si>
     <t>SIS User ID</t>
   </si>
@@ -206,12 +206,6 @@
   </si>
   <si>
     <t>Unposted Final Grade</t>
-  </si>
-  <si>
-    <t>Manual Posting</t>
-  </si>
-  <si>
-    <t>(read only)</t>
   </si>
   <si>
     <t>FA24 - COMP-101-A - CODING ADVENTURES I</t>
@@ -1086,12 +1080,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78BA2EC5-7C9D-4E3C-952F-7434FAB7E38F}">
-  <dimension ref="A1:BJ10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C210D01D-C797-43A6-9753-5A427F7CDB55}">
+  <dimension ref="A1:BJ8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1284,52 +1276,172 @@
       </c>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="AB2" t="s">
+      <c r="A2">
+        <v>62705</v>
+      </c>
+      <c r="B2" t="s">
         <v>62</v>
       </c>
-      <c r="AC2" t="s">
-        <v>62</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>62</v>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>2.89</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="AA2">
+        <v>5</v>
+      </c>
+      <c r="AB2">
+        <v>11</v>
+      </c>
+      <c r="AC2">
+        <v>25</v>
+      </c>
+      <c r="AD2">
+        <v>12</v>
+      </c>
+      <c r="AE2">
+        <v>98.8</v>
+      </c>
+      <c r="AF2">
+        <v>98.8</v>
+      </c>
+      <c r="AG2">
+        <v>24.7</v>
+      </c>
+      <c r="AH2">
+        <v>24.7</v>
+      </c>
+      <c r="AI2">
+        <v>50</v>
+      </c>
+      <c r="AJ2">
+        <v>50</v>
+      </c>
+      <c r="AK2">
+        <v>16.670000000000002</v>
+      </c>
+      <c r="AL2">
+        <v>16.670000000000002</v>
+      </c>
+      <c r="AM2">
+        <v>100</v>
+      </c>
+      <c r="AN2">
+        <v>100</v>
+      </c>
+      <c r="AO2">
+        <v>100</v>
+      </c>
+      <c r="AP2">
+        <v>100</v>
+      </c>
+      <c r="AQ2">
+        <v>102.86</v>
+      </c>
+      <c r="AR2">
+        <v>102.86</v>
+      </c>
+      <c r="AS2">
+        <v>102.86</v>
+      </c>
+      <c r="AT2">
+        <v>102.86</v>
+      </c>
+      <c r="AU2">
+        <v>100</v>
+      </c>
+      <c r="AV2">
+        <v>100</v>
+      </c>
+      <c r="AW2">
+        <v>100</v>
+      </c>
+      <c r="AX2">
+        <v>100</v>
+      </c>
+      <c r="BC2">
+        <v>94.57</v>
+      </c>
+      <c r="BD2">
+        <v>94.57</v>
+      </c>
+      <c r="BE2">
+        <v>63.89</v>
+      </c>
+      <c r="BF2">
+        <v>63.89</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>63</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>63</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>64</v>
+      </c>
+      <c r="BJ2" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>62523</v>
+      </c>
+      <c r="B3" t="s">
+        <v>62</v>
+      </c>
       <c r="C3">
         <v>3</v>
       </c>
       <c r="D3">
-        <v>3</v>
+        <v>2.97</v>
       </c>
       <c r="E3">
         <v>3</v>
       </c>
       <c r="F3">
-        <v>3</v>
+        <v>2.98</v>
       </c>
       <c r="G3">
-        <v>3</v>
+        <v>2.98</v>
       </c>
       <c r="H3">
-        <v>3</v>
+        <v>2.92</v>
       </c>
       <c r="I3">
-        <v>3</v>
+        <v>2.97</v>
       </c>
       <c r="J3">
-        <v>3</v>
+        <v>2.96</v>
       </c>
       <c r="K3">
-        <v>3</v>
+        <v>2.9</v>
       </c>
       <c r="L3">
-        <v>3</v>
+        <v>2.89</v>
       </c>
       <c r="M3">
-        <v>3</v>
+        <v>0.18</v>
       </c>
       <c r="N3">
-        <v>3</v>
+        <v>2.87</v>
       </c>
       <c r="O3">
         <v>1</v>
@@ -1379,89 +1491,77 @@
       <c r="AD3">
         <v>12</v>
       </c>
-      <c r="AE3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AJ3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AN3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AO3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AP3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AQ3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AR3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AS3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AT3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AU3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AV3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AW3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AX3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AY3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AZ3" t="s">
-        <v>63</v>
-      </c>
-      <c r="BA3" t="s">
-        <v>63</v>
-      </c>
-      <c r="BB3" t="s">
-        <v>63</v>
-      </c>
-      <c r="BC3" t="s">
-        <v>63</v>
-      </c>
-      <c r="BD3" t="s">
-        <v>63</v>
-      </c>
-      <c r="BE3" t="s">
-        <v>63</v>
-      </c>
-      <c r="BF3" t="s">
-        <v>63</v>
+      <c r="AE3">
+        <v>90.59</v>
+      </c>
+      <c r="AF3">
+        <v>90.59</v>
+      </c>
+      <c r="AG3">
+        <v>90.59</v>
+      </c>
+      <c r="AH3">
+        <v>90.59</v>
+      </c>
+      <c r="AI3">
+        <v>100</v>
+      </c>
+      <c r="AJ3">
+        <v>100</v>
+      </c>
+      <c r="AK3">
+        <v>100</v>
+      </c>
+      <c r="AL3">
+        <v>100</v>
+      </c>
+      <c r="AM3">
+        <v>100</v>
+      </c>
+      <c r="AN3">
+        <v>100</v>
+      </c>
+      <c r="AO3">
+        <v>100</v>
+      </c>
+      <c r="AP3">
+        <v>100</v>
+      </c>
+      <c r="AQ3">
+        <v>100</v>
+      </c>
+      <c r="AR3">
+        <v>100</v>
+      </c>
+      <c r="AS3">
+        <v>100</v>
+      </c>
+      <c r="AT3">
+        <v>100</v>
+      </c>
+      <c r="AU3">
+        <v>100</v>
+      </c>
+      <c r="AV3">
+        <v>100</v>
+      </c>
+      <c r="AW3">
+        <v>100</v>
+      </c>
+      <c r="AX3">
+        <v>100</v>
+      </c>
+      <c r="BC3">
+        <v>96.61</v>
+      </c>
+      <c r="BD3">
+        <v>96.61</v>
+      </c>
+      <c r="BE3">
+        <v>96.61</v>
+      </c>
+      <c r="BF3">
+        <v>96.61</v>
       </c>
       <c r="BG3" t="s">
         <v>63</v>
@@ -1478,10 +1578,10 @@
     </row>
     <row r="4" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>62705</v>
+        <v>62159</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -1490,25 +1590,73 @@
         <v>3</v>
       </c>
       <c r="E4">
-        <v>2.89</v>
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="I4">
+        <v>3</v>
+      </c>
+      <c r="J4">
+        <v>3</v>
+      </c>
+      <c r="K4">
+        <v>2.97</v>
+      </c>
+      <c r="L4">
+        <v>2.71</v>
+      </c>
+      <c r="N4">
+        <v>2.87</v>
       </c>
       <c r="O4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P4">
         <v>1</v>
       </c>
       <c r="Q4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R4">
+        <v>1</v>
+      </c>
+      <c r="S4">
+        <v>1</v>
+      </c>
+      <c r="T4">
+        <v>1</v>
+      </c>
+      <c r="U4">
+        <v>1</v>
+      </c>
+      <c r="V4">
+        <v>1</v>
+      </c>
+      <c r="W4">
+        <v>1</v>
+      </c>
+      <c r="X4">
+        <v>1</v>
+      </c>
+      <c r="Y4">
+        <v>1</v>
+      </c>
+      <c r="Z4">
         <v>1</v>
       </c>
       <c r="AA4">
         <v>5</v>
       </c>
       <c r="AB4">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AC4">
         <v>25</v>
@@ -1517,28 +1665,28 @@
         <v>12</v>
       </c>
       <c r="AE4">
-        <v>98.8</v>
+        <v>98.62</v>
       </c>
       <c r="AF4">
-        <v>98.8</v>
+        <v>98.62</v>
       </c>
       <c r="AG4">
-        <v>24.7</v>
+        <v>90.4</v>
       </c>
       <c r="AH4">
-        <v>24.7</v>
+        <v>90.4</v>
       </c>
       <c r="AI4">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="AJ4">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="AK4">
-        <v>16.670000000000002</v>
+        <v>100</v>
       </c>
       <c r="AL4">
-        <v>16.670000000000002</v>
+        <v>100</v>
       </c>
       <c r="AM4">
         <v>100</v>
@@ -1553,16 +1701,16 @@
         <v>100</v>
       </c>
       <c r="AQ4">
-        <v>102.86</v>
+        <v>100</v>
       </c>
       <c r="AR4">
-        <v>102.86</v>
+        <v>100</v>
       </c>
       <c r="AS4">
-        <v>102.86</v>
+        <v>100</v>
       </c>
       <c r="AT4">
-        <v>102.86</v>
+        <v>100</v>
       </c>
       <c r="AU4">
         <v>100</v>
@@ -1577,72 +1725,72 @@
         <v>100</v>
       </c>
       <c r="BC4">
-        <v>94.57</v>
+        <v>99.5</v>
       </c>
       <c r="BD4">
-        <v>94.57</v>
+        <v>99.5</v>
       </c>
       <c r="BE4">
-        <v>63.89</v>
+        <v>96.55</v>
       </c>
       <c r="BF4">
-        <v>63.89</v>
+        <v>96.55</v>
       </c>
       <c r="BG4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="BH4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="BI4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="BJ4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>62523</v>
+        <v>8756</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C5">
         <v>3</v>
       </c>
       <c r="D5">
-        <v>2.97</v>
+        <v>3</v>
       </c>
       <c r="E5">
         <v>3</v>
       </c>
       <c r="F5">
-        <v>2.98</v>
+        <v>3</v>
       </c>
       <c r="G5">
-        <v>2.98</v>
+        <v>2.84</v>
       </c>
       <c r="H5">
-        <v>2.92</v>
+        <v>3</v>
       </c>
       <c r="I5">
-        <v>2.97</v>
+        <v>3</v>
       </c>
       <c r="J5">
-        <v>2.96</v>
+        <v>3</v>
       </c>
       <c r="K5">
-        <v>2.9</v>
+        <v>2.87</v>
       </c>
       <c r="L5">
         <v>2.89</v>
       </c>
       <c r="M5">
-        <v>0.18</v>
+        <v>3</v>
       </c>
       <c r="N5">
-        <v>2.87</v>
+        <v>2.73</v>
       </c>
       <c r="O5">
         <v>1</v>
@@ -1693,16 +1841,16 @@
         <v>12</v>
       </c>
       <c r="AE5">
-        <v>90.59</v>
+        <v>98.16</v>
       </c>
       <c r="AF5">
-        <v>90.59</v>
+        <v>98.16</v>
       </c>
       <c r="AG5">
-        <v>90.59</v>
+        <v>98.16</v>
       </c>
       <c r="AH5">
-        <v>90.59</v>
+        <v>98.16</v>
       </c>
       <c r="AI5">
         <v>100</v>
@@ -1753,36 +1901,36 @@
         <v>100</v>
       </c>
       <c r="BC5">
-        <v>96.61</v>
+        <v>99.34</v>
       </c>
       <c r="BD5">
-        <v>96.61</v>
+        <v>99.34</v>
       </c>
       <c r="BE5">
-        <v>96.61</v>
+        <v>99.34</v>
       </c>
       <c r="BF5">
-        <v>96.61</v>
+        <v>99.34</v>
       </c>
       <c r="BG5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="BH5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="BI5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="BJ5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>62159</v>
+        <v>63439</v>
       </c>
       <c r="B6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -1791,31 +1939,34 @@
         <v>3</v>
       </c>
       <c r="E6">
-        <v>3</v>
+        <v>2.95</v>
       </c>
       <c r="F6">
-        <v>3</v>
+        <v>2.68</v>
       </c>
       <c r="G6">
-        <v>3</v>
+        <v>2.4300000000000002</v>
       </c>
       <c r="H6">
-        <v>3</v>
+        <v>2.56</v>
       </c>
       <c r="I6">
-        <v>3</v>
+        <v>2.41</v>
       </c>
       <c r="J6">
-        <v>3</v>
+        <v>2.64</v>
       </c>
       <c r="K6">
-        <v>2.97</v>
+        <v>2.52</v>
       </c>
       <c r="L6">
-        <v>2.71</v>
+        <v>2.46</v>
+      </c>
+      <c r="M6">
+        <v>3</v>
       </c>
       <c r="N6">
-        <v>2.87</v>
+        <v>1.47</v>
       </c>
       <c r="O6">
         <v>1</v>
@@ -1857,25 +2008,25 @@
         <v>5</v>
       </c>
       <c r="AB6">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AC6">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="AD6">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AE6">
-        <v>98.62</v>
+        <v>86.39</v>
       </c>
       <c r="AF6">
-        <v>98.62</v>
+        <v>86.39</v>
       </c>
       <c r="AG6">
-        <v>90.4</v>
+        <v>86.39</v>
       </c>
       <c r="AH6">
-        <v>90.4</v>
+        <v>86.39</v>
       </c>
       <c r="AI6">
         <v>100</v>
@@ -1902,40 +2053,40 @@
         <v>100</v>
       </c>
       <c r="AQ6">
-        <v>100</v>
+        <v>68.569999999999993</v>
       </c>
       <c r="AR6">
-        <v>100</v>
+        <v>68.569999999999993</v>
       </c>
       <c r="AS6">
-        <v>100</v>
+        <v>68.569999999999993</v>
       </c>
       <c r="AT6">
-        <v>100</v>
+        <v>68.569999999999993</v>
       </c>
       <c r="AU6">
-        <v>100</v>
+        <v>91.67</v>
       </c>
       <c r="AV6">
-        <v>100</v>
+        <v>91.67</v>
       </c>
       <c r="AW6">
-        <v>100</v>
+        <v>91.67</v>
       </c>
       <c r="AX6">
-        <v>100</v>
+        <v>91.67</v>
       </c>
       <c r="BC6">
-        <v>99.5</v>
+        <v>83.1</v>
       </c>
       <c r="BD6">
-        <v>99.5</v>
+        <v>83.1</v>
       </c>
       <c r="BE6">
-        <v>96.55</v>
+        <v>83.1</v>
       </c>
       <c r="BF6">
-        <v>96.55</v>
+        <v>83.1</v>
       </c>
       <c r="BG6" t="s">
         <v>65</v>
@@ -1952,10 +2103,10 @@
     </row>
     <row r="7" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>8756</v>
+        <v>10325</v>
       </c>
       <c r="B7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C7">
         <v>3</v>
@@ -1964,34 +2115,31 @@
         <v>3</v>
       </c>
       <c r="E7">
-        <v>3</v>
+        <v>2.84</v>
       </c>
       <c r="F7">
-        <v>3</v>
+        <v>2.64</v>
       </c>
       <c r="G7">
-        <v>2.84</v>
+        <v>2.4300000000000002</v>
       </c>
       <c r="H7">
-        <v>3</v>
+        <v>2.6</v>
       </c>
       <c r="I7">
-        <v>3</v>
+        <v>2.44</v>
       </c>
       <c r="J7">
-        <v>3</v>
+        <v>2.64</v>
       </c>
       <c r="K7">
-        <v>2.87</v>
+        <v>2.48</v>
       </c>
       <c r="L7">
-        <v>2.89</v>
-      </c>
-      <c r="M7">
-        <v>3</v>
+        <v>2.4900000000000002</v>
       </c>
       <c r="N7">
-        <v>2.73</v>
+        <v>1.47</v>
       </c>
       <c r="O7">
         <v>1</v>
@@ -2005,28 +2153,7 @@
       <c r="R7">
         <v>1</v>
       </c>
-      <c r="S7">
-        <v>1</v>
-      </c>
-      <c r="T7">
-        <v>1</v>
-      </c>
-      <c r="U7">
-        <v>1</v>
-      </c>
       <c r="V7">
-        <v>1</v>
-      </c>
-      <c r="W7">
-        <v>1</v>
-      </c>
-      <c r="X7">
-        <v>1</v>
-      </c>
-      <c r="Y7">
-        <v>1</v>
-      </c>
-      <c r="Z7">
         <v>1</v>
       </c>
       <c r="AA7">
@@ -2042,16 +2169,16 @@
         <v>12</v>
       </c>
       <c r="AE7">
-        <v>98.16</v>
+        <v>84.95</v>
       </c>
       <c r="AF7">
-        <v>98.16</v>
+        <v>84.95</v>
       </c>
       <c r="AG7">
-        <v>98.16</v>
+        <v>77.87</v>
       </c>
       <c r="AH7">
-        <v>98.16</v>
+        <v>77.87</v>
       </c>
       <c r="AI7">
         <v>100</v>
@@ -2060,10 +2187,10 @@
         <v>100</v>
       </c>
       <c r="AK7">
-        <v>100</v>
+        <v>41.67</v>
       </c>
       <c r="AL7">
-        <v>100</v>
+        <v>41.67</v>
       </c>
       <c r="AM7">
         <v>100</v>
@@ -2102,22 +2229,22 @@
         <v>100</v>
       </c>
       <c r="BC7">
-        <v>99.34</v>
+        <v>94.58</v>
       </c>
       <c r="BD7">
-        <v>99.34</v>
+        <v>94.58</v>
       </c>
       <c r="BE7">
-        <v>99.34</v>
+        <v>85.03</v>
       </c>
       <c r="BF7">
-        <v>99.34</v>
+        <v>85.03</v>
       </c>
       <c r="BG7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="BH7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="BI7" t="s">
         <v>65</v>
@@ -2127,378 +2254,50 @@
       </c>
     </row>
     <row r="8" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>63439</v>
-      </c>
       <c r="B8" t="s">
-        <v>64</v>
-      </c>
-      <c r="C8">
-        <v>3</v>
-      </c>
-      <c r="D8">
-        <v>3</v>
-      </c>
-      <c r="E8">
-        <v>2.95</v>
-      </c>
-      <c r="F8">
-        <v>2.68</v>
-      </c>
-      <c r="G8">
-        <v>2.4300000000000002</v>
-      </c>
-      <c r="H8">
-        <v>2.56</v>
-      </c>
-      <c r="I8">
-        <v>2.41</v>
-      </c>
-      <c r="J8">
-        <v>2.64</v>
-      </c>
-      <c r="K8">
-        <v>2.52</v>
-      </c>
-      <c r="L8">
-        <v>2.46</v>
-      </c>
-      <c r="M8">
-        <v>3</v>
-      </c>
-      <c r="N8">
-        <v>1.47</v>
-      </c>
-      <c r="O8">
-        <v>1</v>
-      </c>
-      <c r="P8">
-        <v>1</v>
-      </c>
-      <c r="Q8">
-        <v>1</v>
-      </c>
-      <c r="R8">
-        <v>1</v>
-      </c>
-      <c r="S8">
-        <v>1</v>
-      </c>
-      <c r="T8">
-        <v>1</v>
-      </c>
-      <c r="U8">
-        <v>1</v>
-      </c>
-      <c r="V8">
-        <v>1</v>
-      </c>
-      <c r="W8">
-        <v>1</v>
-      </c>
-      <c r="X8">
-        <v>1</v>
-      </c>
-      <c r="Y8">
-        <v>1</v>
-      </c>
-      <c r="Z8">
-        <v>1</v>
-      </c>
-      <c r="AA8">
-        <v>5</v>
-      </c>
-      <c r="AB8">
-        <v>9</v>
-      </c>
-      <c r="AC8">
-        <v>15</v>
-      </c>
-      <c r="AD8">
-        <v>11</v>
-      </c>
-      <c r="AE8">
-        <v>86.39</v>
-      </c>
-      <c r="AF8">
-        <v>86.39</v>
+        <v>62</v>
       </c>
       <c r="AG8">
-        <v>86.39</v>
+        <v>0</v>
       </c>
       <c r="AH8">
-        <v>86.39</v>
-      </c>
-      <c r="AI8">
-        <v>100</v>
-      </c>
-      <c r="AJ8">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="AK8">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="AL8">
-        <v>100</v>
-      </c>
-      <c r="AM8">
-        <v>100</v>
-      </c>
-      <c r="AN8">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="AO8">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="AP8">
-        <v>100</v>
-      </c>
-      <c r="AQ8">
-        <v>68.569999999999993</v>
-      </c>
-      <c r="AR8">
-        <v>68.569999999999993</v>
+        <v>0</v>
       </c>
       <c r="AS8">
-        <v>68.569999999999993</v>
+        <v>0</v>
       </c>
       <c r="AT8">
-        <v>68.569999999999993</v>
-      </c>
-      <c r="AU8">
-        <v>91.67</v>
-      </c>
-      <c r="AV8">
-        <v>91.67</v>
+        <v>0</v>
       </c>
       <c r="AW8">
-        <v>91.67</v>
+        <v>0</v>
       </c>
       <c r="AX8">
-        <v>91.67</v>
-      </c>
-      <c r="BC8">
-        <v>83.1</v>
-      </c>
-      <c r="BD8">
-        <v>83.1</v>
+        <v>0</v>
       </c>
       <c r="BE8">
-        <v>83.1</v>
+        <v>0</v>
       </c>
       <c r="BF8">
-        <v>83.1</v>
-      </c>
-      <c r="BG8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BH8" t="s">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="BI8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="BJ8" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="9" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>10325</v>
-      </c>
-      <c r="B9" t="s">
-        <v>64</v>
-      </c>
-      <c r="C9">
-        <v>3</v>
-      </c>
-      <c r="D9">
-        <v>3</v>
-      </c>
-      <c r="E9">
-        <v>2.84</v>
-      </c>
-      <c r="F9">
-        <v>2.64</v>
-      </c>
-      <c r="G9">
-        <v>2.4300000000000002</v>
-      </c>
-      <c r="H9">
-        <v>2.6</v>
-      </c>
-      <c r="I9">
-        <v>2.44</v>
-      </c>
-      <c r="J9">
-        <v>2.64</v>
-      </c>
-      <c r="K9">
-        <v>2.48</v>
-      </c>
-      <c r="L9">
-        <v>2.4900000000000002</v>
-      </c>
-      <c r="N9">
-        <v>1.47</v>
-      </c>
-      <c r="O9">
-        <v>1</v>
-      </c>
-      <c r="P9">
-        <v>1</v>
-      </c>
-      <c r="Q9">
-        <v>1</v>
-      </c>
-      <c r="R9">
-        <v>1</v>
-      </c>
-      <c r="V9">
-        <v>1</v>
-      </c>
-      <c r="AA9">
-        <v>5</v>
-      </c>
-      <c r="AB9">
-        <v>10</v>
-      </c>
-      <c r="AC9">
-        <v>25</v>
-      </c>
-      <c r="AD9">
-        <v>12</v>
-      </c>
-      <c r="AE9">
-        <v>84.95</v>
-      </c>
-      <c r="AF9">
-        <v>84.95</v>
-      </c>
-      <c r="AG9">
-        <v>77.87</v>
-      </c>
-      <c r="AH9">
-        <v>77.87</v>
-      </c>
-      <c r="AI9">
-        <v>100</v>
-      </c>
-      <c r="AJ9">
-        <v>100</v>
-      </c>
-      <c r="AK9">
-        <v>41.67</v>
-      </c>
-      <c r="AL9">
-        <v>41.67</v>
-      </c>
-      <c r="AM9">
-        <v>100</v>
-      </c>
-      <c r="AN9">
-        <v>100</v>
-      </c>
-      <c r="AO9">
-        <v>100</v>
-      </c>
-      <c r="AP9">
-        <v>100</v>
-      </c>
-      <c r="AQ9">
-        <v>100</v>
-      </c>
-      <c r="AR9">
-        <v>100</v>
-      </c>
-      <c r="AS9">
-        <v>100</v>
-      </c>
-      <c r="AT9">
-        <v>100</v>
-      </c>
-      <c r="AU9">
-        <v>100</v>
-      </c>
-      <c r="AV9">
-        <v>100</v>
-      </c>
-      <c r="AW9">
-        <v>100</v>
-      </c>
-      <c r="AX9">
-        <v>100</v>
-      </c>
-      <c r="BC9">
-        <v>94.58</v>
-      </c>
-      <c r="BD9">
-        <v>94.58</v>
-      </c>
-      <c r="BE9">
-        <v>85.03</v>
-      </c>
-      <c r="BF9">
-        <v>85.03</v>
-      </c>
-      <c r="BG9" t="s">
-        <v>65</v>
-      </c>
-      <c r="BH9" t="s">
-        <v>65</v>
-      </c>
-      <c r="BI9" t="s">
-        <v>67</v>
-      </c>
-      <c r="BJ9" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="10" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>64</v>
-      </c>
-      <c r="AG10">
-        <v>0</v>
-      </c>
-      <c r="AH10">
-        <v>0</v>
-      </c>
-      <c r="AK10">
-        <v>0</v>
-      </c>
-      <c r="AL10">
-        <v>0</v>
-      </c>
-      <c r="AO10">
-        <v>0</v>
-      </c>
-      <c r="AP10">
-        <v>0</v>
-      </c>
-      <c r="AS10">
-        <v>0</v>
-      </c>
-      <c r="AT10">
-        <v>0</v>
-      </c>
-      <c r="AW10">
-        <v>0</v>
-      </c>
-      <c r="AX10">
-        <v>0</v>
-      </c>
-      <c r="BE10">
-        <v>0</v>
-      </c>
-      <c r="BF10">
-        <v>0</v>
-      </c>
-      <c r="BI10" t="s">
-        <v>68</v>
-      </c>
-      <c r="BJ10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>